<commit_message>
atualiza scripts e adiciona completude geral
</commit_message>
<xml_diff>
--- a/planilhas_teste.xlsx
+++ b/planilhas_teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\PYTHON\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7110E933-F35A-444B-8DCB-287B645BCDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83474D36-13D7-403C-961C-881304D30E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="20">
-  <si>
-    <t>TITULO DA TABELA</t>
-  </si>
-  <si>
-    <t>PERIODO</t>
-  </si>
-  <si>
-    <t>PERIODO_ANALISADO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
   <si>
     <t>CABECALHO_1</t>
   </si>
@@ -98,6 +89,24 @@
   </si>
   <si>
     <t>ERRO</t>
+  </si>
+  <si>
+    <t>PERÍODO</t>
+  </si>
+  <si>
+    <t>PERÍODO_ANALISADO</t>
+  </si>
+  <si>
+    <t>PLANILHA 1</t>
+  </si>
+  <si>
+    <t>PLANILHA 2</t>
+  </si>
+  <si>
+    <t>PLANILHA 3</t>
+  </si>
+  <si>
+    <t>PLANILHA 4</t>
   </si>
 </sst>
 </file>
@@ -438,9 +447,7 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="A1:J12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -451,44 +458,44 @@
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -496,31 +503,31 @@
         <v>2017</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -528,22 +535,22 @@
         <v>2018</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -560,10 +567,10 @@
         <v>2019</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -572,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -584,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -604,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -636,10 +643,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -668,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
@@ -700,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -749,7 +756,7 @@
     </row>
     <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -761,9 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA4AED9-A175-4FEC-8A2A-AB367AE205B7}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -773,35 +778,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -812,16 +817,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
@@ -855,7 +860,7 @@
         <v>2022</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -864,13 +869,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -887,10 +892,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -901,10 +906,10 @@
         <v>2024</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -913,15 +918,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -933,9 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E25E0C5-D39B-4F5E-AEA0-FCF3A03EDFCE}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -945,26 +948,26 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -975,10 +978,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,13 +1003,13 @@
         <v>2022</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,12 +1023,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1037,9 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71240775-5127-47DF-86C8-864D123FC62F}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1048,50 +1049,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1099,31 +1100,31 @@
         <v>2017</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1131,22 +1132,22 @@
         <v>2018</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -1163,10 +1164,10 @@
         <v>2019</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1175,10 +1176,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1187,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1207,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -1239,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
@@ -1271,10 +1272,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -1303,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
@@ -1352,7 +1353,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1364,20 +1365,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F14326B-828F-4D00-AC1A-CE1375604733}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6E0BFC-7128-429D-8F46-78459044652F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1397,12 +1396,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>